<commit_message>
testing variations of membership functions in fuzzy inference system cred, final configuration complete
</commit_message>
<xml_diff>
--- a/FIS/cred/NATO_STANAG_2511.xlsx
+++ b/FIS/cred/NATO_STANAG_2511.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Desktop\fuzzy_cw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FC4729F-C7EF-4BDA-A4EF-B5F429117525}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D6753E8-754C-4007-9BFE-4A5CD30E5CAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="645" yWindow="3510" windowWidth="15015" windowHeight="19215" xr2:uid="{E9DBF028-2AFF-4D1D-8975-9DD69804B774}"/>
+    <workbookView xWindow="2205" yWindow="2205" windowWidth="21600" windowHeight="11385" xr2:uid="{E9DBF028-2AFF-4D1D-8975-9DD69804B774}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -63,19 +63,19 @@
     <t>B</t>
   </si>
   <si>
-    <t>Expected</t>
-  </si>
-  <si>
-    <t>rel Output</t>
-  </si>
-  <si>
     <t>gut(%)</t>
   </si>
   <si>
-    <t>Validations(0- 30)</t>
-  </si>
-  <si>
-    <t>cred Output</t>
+    <t>Expected reliability grade</t>
+  </si>
+  <si>
+    <t>Validations(0-10)</t>
+  </si>
+  <si>
+    <t>Credibility (1-6) centroid</t>
+  </si>
+  <si>
+    <t>Reliability (A-F)</t>
   </si>
 </sst>
 </file>
@@ -443,7 +443,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E52529AF-6C54-48C1-85E9-720B2510375C}">
   <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
@@ -451,13 +451,14 @@
   <cols>
     <col min="1" max="2" width="17.85546875" customWidth="1"/>
     <col min="3" max="3" width="2.140625" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" customWidth="1"/>
+    <col min="4" max="4" width="25.28515625" customWidth="1"/>
     <col min="5" max="5" width="2.42578125" customWidth="1"/>
-    <col min="6" max="6" width="18.42578125" customWidth="1"/>
-    <col min="7" max="7" width="4.28515625" customWidth="1"/>
+    <col min="6" max="6" width="28.85546875" customWidth="1"/>
+    <col min="7" max="7" width="2.42578125" customWidth="1"/>
     <col min="8" max="9" width="18.5703125" customWidth="1"/>
     <col min="10" max="10" width="2" customWidth="1"/>
-    <col min="11" max="11" width="22.5703125" customWidth="1"/>
+    <col min="11" max="11" width="25.42578125" customWidth="1"/>
+    <col min="12" max="12" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -469,22 +470,22 @@
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G1" s="2"/>
       <c r="H1" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="J1" s="2"/>
       <c r="K1" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -502,18 +503,18 @@
       </c>
       <c r="E2" s="3"/>
       <c r="F2">
-        <v>6</v>
+        <v>6.3154569402055438</v>
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I2" s="3">
         <v>4</v>
       </c>
       <c r="J2" s="3"/>
-      <c r="K2">
-        <v>3.4712214541201076</v>
+      <c r="K2" s="3">
+        <v>3.1686975605229013</v>
       </c>
       <c r="L2" s="3"/>
     </row>
@@ -530,18 +531,18 @@
       </c>
       <c r="E3" s="3"/>
       <c r="F3">
-        <v>6</v>
+        <v>6.2564160067025645</v>
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I3" s="3">
         <v>8</v>
       </c>
       <c r="J3" s="3"/>
-      <c r="K3">
-        <v>3.4266740895709131</v>
+      <c r="K3" s="3">
+        <v>2.7706313888264562</v>
       </c>
       <c r="L3" s="3"/>
     </row>
@@ -562,14 +563,14 @@
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I4" s="3">
         <v>12</v>
       </c>
       <c r="J4" s="3"/>
-      <c r="K4">
-        <v>3.935437795700985</v>
+      <c r="K4" s="3">
+        <v>3.5389689214470712</v>
       </c>
       <c r="L4" s="3"/>
     </row>
@@ -590,14 +591,14 @@
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="3">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I5" s="3">
         <v>16</v>
       </c>
       <c r="J5" s="3"/>
-      <c r="K5">
-        <v>4.063446124000528</v>
+      <c r="K5" s="3">
+        <v>3.9583081450558426</v>
       </c>
       <c r="L5" s="3"/>
     </row>
@@ -618,14 +619,14 @@
       </c>
       <c r="G6" s="3"/>
       <c r="H6" s="3">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="I6" s="3">
         <v>20</v>
       </c>
       <c r="J6" s="3"/>
-      <c r="K6">
-        <v>4.0215633997925408</v>
+      <c r="K6" s="3">
+        <v>3.4269002284580381</v>
       </c>
       <c r="L6" s="3"/>
     </row>
@@ -646,14 +647,14 @@
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="3">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="I7" s="3">
         <v>24</v>
       </c>
       <c r="J7" s="3"/>
-      <c r="K7">
-        <v>4.0385039176156017</v>
+      <c r="K7" s="3">
+        <v>2.8255265341804496</v>
       </c>
       <c r="L7" s="3"/>
     </row>
@@ -674,14 +675,14 @@
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="3">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="I8" s="3">
         <v>28</v>
       </c>
       <c r="J8" s="3"/>
-      <c r="K8">
-        <v>5.1969909721368008</v>
+      <c r="K8" s="3">
+        <v>3.2731999206807356</v>
       </c>
       <c r="L8" s="3"/>
     </row>
@@ -702,14 +703,14 @@
       </c>
       <c r="G9" s="3"/>
       <c r="H9" s="3">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="I9" s="3">
         <v>32</v>
       </c>
       <c r="J9" s="3"/>
-      <c r="K9">
-        <v>5.2193041581252704</v>
+      <c r="K9" s="3">
+        <v>2.4171065606495308</v>
       </c>
       <c r="L9" s="3"/>
     </row>
@@ -730,14 +731,14 @@
       </c>
       <c r="G10" s="3"/>
       <c r="H10" s="3">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="I10" s="3">
         <v>36</v>
       </c>
       <c r="J10" s="3"/>
-      <c r="K10">
-        <v>5.2212284708270778</v>
+      <c r="K10" s="3">
+        <v>1.6072375787589124</v>
       </c>
       <c r="L10" s="3"/>
     </row>
@@ -755,13 +756,14 @@
         <v>1.5278696036486905</v>
       </c>
       <c r="H11" s="3">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I11" s="3">
         <v>40</v>
       </c>
-      <c r="K11">
-        <v>5.1233757604194725</v>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3">
+        <v>1.2033260647614508</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -778,13 +780,14 @@
         <v>1.489834292864558</v>
       </c>
       <c r="H12" s="3">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="I12" s="3">
         <v>44</v>
       </c>
-      <c r="K12">
-        <v>5.0670488488462233</v>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3">
+        <v>5.2296748276832883</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -801,13 +804,14 @@
         <v>3.9998977394245094</v>
       </c>
       <c r="H13" s="3">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="I13" s="3">
         <v>48</v>
       </c>
-      <c r="K13">
-        <v>3.6846085600087388</v>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3">
+        <v>4.1875637142994426</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -824,13 +828,14 @@
         <v>4.0001703709594914</v>
       </c>
       <c r="H14" s="3">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="I14" s="3">
         <v>52</v>
       </c>
-      <c r="K14">
-        <v>3.0008509534638845</v>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3">
+        <v>3.9437001617800607</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -847,13 +852,14 @@
         <v>4.0071375453924754</v>
       </c>
       <c r="H15" s="3">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="I15" s="3">
         <v>56</v>
       </c>
-      <c r="K15">
-        <v>2.5060937361456244</v>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3">
+        <v>3.5727161545206436</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -870,13 +876,14 @@
         <v>4.3176217996932298</v>
       </c>
       <c r="H16" s="3">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="I16" s="3">
         <v>60</v>
       </c>
-      <c r="K16">
-        <v>2.2192145132067935</v>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3">
+        <v>3.0320946589444913</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -893,13 +900,14 @@
         <v>4.9293799353882441</v>
       </c>
       <c r="H17" s="3">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="I17" s="3">
         <v>64</v>
       </c>
-      <c r="K17">
-        <v>1.630744653778132</v>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3">
+        <v>1.807468902175442</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -916,13 +924,14 @@
         <v>4.9993249428934421</v>
       </c>
       <c r="H18" s="3">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="I18" s="3">
         <v>68</v>
       </c>
-      <c r="K18">
-        <v>1.4649212700406997</v>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3">
+        <v>1.3363942218683218</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -939,13 +948,14 @@
         <v>5.0826092704683719</v>
       </c>
       <c r="H19" s="3">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="I19" s="3">
         <v>72</v>
       </c>
-      <c r="K19">
-        <v>1.223921860039122</v>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3">
+        <v>0.9983021048316667</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -962,13 +972,14 @@
         <v>5.8450093797485856</v>
       </c>
       <c r="H20" s="3">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="I20" s="3">
         <v>76</v>
       </c>
-      <c r="K20">
-        <v>1.223921860039122</v>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3">
+        <v>0.74578295007492323</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -982,16 +993,17 @@
         <v>3</v>
       </c>
       <c r="F21">
-        <v>6</v>
+        <v>6.2215316031519983</v>
       </c>
       <c r="H21" s="3">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="I21" s="3">
         <v>80</v>
       </c>
-      <c r="K21">
-        <v>1.223921860039122</v>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3">
+        <v>0.69916048646939877</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
@@ -1005,16 +1017,17 @@
         <v>3</v>
       </c>
       <c r="F22">
-        <v>6</v>
+        <v>6.2886491400835389</v>
       </c>
       <c r="H22" s="3">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="I22" s="3">
         <v>84</v>
       </c>
-      <c r="K22">
-        <v>1.223921860039122</v>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3">
+        <v>1.1006231168362968</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
@@ -1031,13 +1044,14 @@
         <v>3.3324329786581037</v>
       </c>
       <c r="H23" s="3">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="I23" s="3">
         <v>88</v>
       </c>
-      <c r="K23">
-        <v>1.223921860039122</v>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3">
+        <v>3.3346065793099666</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
@@ -1054,13 +1068,14 @@
         <v>3.8340643814578548</v>
       </c>
       <c r="H24" s="3">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="I24" s="3">
         <v>92</v>
       </c>
-      <c r="K24">
-        <v>1.223921860039122</v>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3">
+        <v>2.3207382788713429</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
@@ -1077,13 +1092,14 @@
         <v>3.3594028761362651</v>
       </c>
       <c r="H25" s="3">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="I25" s="3">
         <v>96</v>
       </c>
-      <c r="K25">
-        <v>1.223921860039122</v>
+      <c r="J25" s="3"/>
+      <c r="K25" s="3">
+        <v>2.0241123479739231</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
@@ -1100,13 +1116,14 @@
         <v>1.8576174232931988</v>
       </c>
       <c r="H26" s="3">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="I26" s="3">
         <v>100</v>
       </c>
-      <c r="K26">
-        <v>1.223921860039122</v>
+      <c r="J26" s="3"/>
+      <c r="K26" s="3">
+        <v>1.7236265462102696</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
@@ -1123,13 +1140,14 @@
         <v>1.469450867254618</v>
       </c>
       <c r="H27" s="3">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="I27" s="3">
         <v>100</v>
       </c>
-      <c r="K27">
-        <v>1.223921860039122</v>
+      <c r="J27" s="3"/>
+      <c r="K27" s="3">
+        <v>1.2699848065226138</v>
       </c>
     </row>
   </sheetData>

</xml_diff>